<commit_message>
add cplex, gurobi, ortools
</commit_message>
<xml_diff>
--- a/CSP.xlsx
+++ b/CSP.xlsx
@@ -478,7 +478,7 @@
         <v>28860</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2808271699996112</v>
+        <v>0.213964613</v>
       </c>
       <c r="E2" t="n">
         <v>4</v>
@@ -502,7 +502,7 @@
         <v>238840</v>
       </c>
       <c r="D3" t="n">
-        <v>18.9492616890002</v>
+        <v>16.44030466</v>
       </c>
       <c r="E3" t="n">
         <v>6</v>
@@ -526,7 +526,7 @@
         <v>818706</v>
       </c>
       <c r="D4" t="n">
-        <v>18.12764739999875</v>
+        <v>11.2207408</v>
       </c>
       <c r="E4" t="n">
         <v>9</v>
@@ -550,7 +550,7 @@
         <v>1796500</v>
       </c>
       <c r="D5" t="n">
-        <v>53.77896598799998</v>
+        <v>37.39759781</v>
       </c>
       <c r="E5" t="n">
         <v>11</v>
@@ -574,7 +574,7 @@
         <v>3592984</v>
       </c>
       <c r="D6" t="n">
-        <v>104.7065740160015</v>
+        <v>70.94194152999999</v>
       </c>
       <c r="E6" t="n">
         <v>14</v>
@@ -598,7 +598,7 @@
         <v>174888</v>
       </c>
       <c r="D7" t="n">
-        <v>1.348582016000364</v>
+        <v>0.774997429</v>
       </c>
       <c r="E7" t="n">
         <v>2</v>
@@ -622,7 +622,7 @@
         <v>1061604</v>
       </c>
       <c r="D8" t="n">
-        <v>23.09903953399953</v>
+        <v>13.67573711</v>
       </c>
       <c r="E8" t="n">
         <v>3</v>
@@ -646,7 +646,7 @@
         <v>3994824</v>
       </c>
       <c r="D9" t="n">
-        <v>41.93528675000016</v>
+        <v>27.53228301</v>
       </c>
       <c r="E9" t="n">
         <v>5</v>
@@ -670,7 +670,7 @@
         <v>8592395</v>
       </c>
       <c r="D10" t="n">
-        <v>180.1803227929995</v>
+        <v>72.41773309</v>
       </c>
       <c r="E10" t="n">
         <v>6</v>
@@ -694,7 +694,7 @@
         <v>15698958</v>
       </c>
       <c r="D11" t="n">
-        <v>414.3813663300007</v>
+        <v>190.7715986</v>
       </c>
       <c r="E11" t="n">
         <v>7</v>
@@ -708,92 +708,92 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ngcut1</t>
+          <t>WANG1</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>319</v>
+        <v>6340</v>
       </c>
       <c r="C12" t="n">
-        <v>2391</v>
+        <v>1193326</v>
       </c>
       <c r="D12" t="n">
-        <v>0.02132156500010751</v>
+        <v>33.34636053</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>COMPLETE</t>
+          <t>TIMEOUT</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ngcut2</t>
+          <t>WANG2</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>805</v>
+        <v>6550</v>
       </c>
       <c r="C13" t="n">
-        <v>10834</v>
+        <v>1115244</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1576840809993882</v>
+        <v>31.96047847</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>COMPLETE</t>
+          <t>TIMEOUT</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ngcut3</t>
+          <t>WANG3</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1191</v>
+        <v>6592</v>
       </c>
       <c r="C14" t="n">
-        <v>18366</v>
+        <v>1132506</v>
       </c>
       <c r="D14" t="n">
-        <v>0.1865207030004967</v>
+        <v>11.4881725</v>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>COMPLETE</t>
+          <t>TIMEOUT</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ngcut4</t>
+          <t>ngcut1</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>194</v>
+        <v>319</v>
       </c>
       <c r="C15" t="n">
-        <v>1318</v>
+        <v>2391</v>
       </c>
       <c r="D15" t="n">
-        <v>0.005960083999525523</v>
+        <v>0.017789558</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -804,20 +804,20 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ngcut5</t>
+          <t>ngcut2</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>597</v>
+        <v>805</v>
       </c>
       <c r="C16" t="n">
-        <v>8025</v>
+        <v>10834</v>
       </c>
       <c r="D16" t="n">
-        <v>0.04054832300062117</v>
+        <v>0.137762133</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -828,17 +828,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ngcut6</t>
+          <t>ngcut3</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>701</v>
+        <v>1191</v>
       </c>
       <c r="C17" t="n">
-        <v>7549</v>
+        <v>18366</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1569921020000038</v>
+        <v>0.150790223</v>
       </c>
       <c r="E17" t="n">
         <v>3</v>
@@ -852,20 +852,20 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>ngcut7</t>
+          <t>ngcut4</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>356</v>
+        <v>194</v>
       </c>
       <c r="C18" t="n">
-        <v>1924</v>
+        <v>1318</v>
       </c>
       <c r="D18" t="n">
-        <v>0.01294073499957449</v>
+        <v>0.004480143</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -876,20 +876,20 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>ngcut8</t>
+          <t>ngcut5</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>676</v>
+        <v>597</v>
       </c>
       <c r="C19" t="n">
-        <v>8658</v>
+        <v>8025</v>
       </c>
       <c r="D19" t="n">
-        <v>0.02944504399965808</v>
+        <v>0.024679722</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -900,72 +900,72 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>WANG1</t>
+          <t>ngcut6</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>6340</v>
+        <v>701</v>
       </c>
       <c r="C20" t="n">
-        <v>1193326</v>
+        <v>7549</v>
       </c>
       <c r="D20" t="n">
-        <v>44.20853379300024</v>
+        <v>0.122805094</v>
       </c>
       <c r="E20" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>TIMEOUT</t>
+          <t>COMPLETE</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>WANG2</t>
+          <t>ngcut7</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>6550</v>
+        <v>356</v>
       </c>
       <c r="C21" t="n">
-        <v>1115244</v>
+        <v>1924</v>
       </c>
       <c r="D21" t="n">
-        <v>53.81764915299937</v>
+        <v>0.006977101</v>
       </c>
       <c r="E21" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>TIMEOUT</t>
+          <t>COMPLETE</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>WANG3</t>
+          <t>ngcut8</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>6592</v>
+        <v>676</v>
       </c>
       <c r="C22" t="n">
-        <v>1132506</v>
+        <v>8658</v>
       </c>
       <c r="D22" t="n">
-        <v>26.47194833799949</v>
+        <v>0.026513081</v>
       </c>
       <c r="E22" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>TIMEOUT</t>
+          <t>COMPLETE</t>
         </is>
       </c>
     </row>
@@ -982,7 +982,7 @@
         <v>24783</v>
       </c>
       <c r="D23" t="n">
-        <v>0.4283502039997984</v>
+        <v>0.180434531</v>
       </c>
       <c r="E23" t="n">
         <v>3</v>
@@ -1006,7 +1006,7 @@
         <v>9658</v>
       </c>
       <c r="D24" t="n">
-        <v>0.2797023170005559</v>
+        <v>0.156260539</v>
       </c>
       <c r="E24" t="n">
         <v>3</v>
@@ -1030,7 +1030,7 @@
         <v>16742</v>
       </c>
       <c r="D25" t="n">
-        <v>0.2526784840010805</v>
+        <v>0.140559098</v>
       </c>
       <c r="E25" t="n">
         <v>2</v>
@@ -1054,7 +1054,7 @@
         <v>52261</v>
       </c>
       <c r="D26" t="n">
-        <v>0.913888990000487</v>
+        <v>0.385654115</v>
       </c>
       <c r="E26" t="n">
         <v>3</v>
@@ -1078,7 +1078,7 @@
         <v>9852</v>
       </c>
       <c r="D27" t="n">
-        <v>0.05479677800030913</v>
+        <v>0.031486081</v>
       </c>
       <c r="E27" t="n">
         <v>2</v>
@@ -1102,7 +1102,7 @@
         <v>86188</v>
       </c>
       <c r="D28" t="n">
-        <v>0.7838106489998609</v>
+        <v>0.318296757</v>
       </c>
       <c r="E28" t="n">
         <v>2</v>
@@ -1126,7 +1126,7 @@
         <v>4536751</v>
       </c>
       <c r="D29" t="n">
-        <v>21.92716156800088</v>
+        <v>9.334168258</v>
       </c>
       <c r="E29" t="n">
         <v>24</v>
@@ -1150,7 +1150,7 @@
         <v>4309505</v>
       </c>
       <c r="D30" t="n">
-        <v>29.00481746500009</v>
+        <v>8.694348646</v>
       </c>
       <c r="E30" t="n">
         <v>23</v>
@@ -1174,7 +1174,7 @@
         <v>1987594</v>
       </c>
       <c r="D31" t="n">
-        <v>76.87314971699925</v>
+        <v>32.14191192</v>
       </c>
       <c r="E31" t="n">
         <v>11</v>
@@ -1198,7 +1198,7 @@
         <v>1430809</v>
       </c>
       <c r="D32" t="n">
-        <v>30.35248784999931</v>
+        <v>8.296645525000001</v>
       </c>
       <c r="E32" t="n">
         <v>8</v>
@@ -1222,7 +1222,7 @@
         <v>534395</v>
       </c>
       <c r="D33" t="n">
-        <v>11.8057477700022</v>
+        <v>3.330431542</v>
       </c>
       <c r="E33" t="n">
         <v>5</v>
@@ -1246,7 +1246,7 @@
         <v>1321779</v>
       </c>
       <c r="D34" t="n">
-        <v>178.8120703460008</v>
+        <v>55.65743394</v>
       </c>
       <c r="E34" t="n">
         <v>4</v>
@@ -1270,7 +1270,7 @@
         <v>105623</v>
       </c>
       <c r="D35" t="n">
-        <v>1.135583628998575</v>
+        <v>0.424607828</v>
       </c>
       <c r="E35" t="n">
         <v>2</v>
@@ -1294,7 +1294,7 @@
         <v>3285792</v>
       </c>
       <c r="D36" t="n">
-        <v>73.60113360999821</v>
+        <v>25.69063781</v>
       </c>
       <c r="E36" t="n">
         <v>6</v>
@@ -1308,20 +1308,20 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>CHL2</t>
+          <t>CHL3</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>2242</v>
+        <v>11121</v>
       </c>
       <c r="C37" t="n">
-        <v>83220</v>
+        <v>305340</v>
       </c>
       <c r="D37" t="n">
-        <v>1.442656093000551</v>
+        <v>2.293431980004243</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -1332,17 +1332,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>CHL3</t>
+          <t>CHL4</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>11121</v>
+        <v>12062</v>
       </c>
       <c r="C38" t="n">
-        <v>305340</v>
+        <v>287415</v>
       </c>
       <c r="D38" t="n">
-        <v>7.889073136000661</v>
+        <v>2.424728341000446</v>
       </c>
       <c r="E38" t="n">
         <v>1</v>
@@ -1356,20 +1356,20 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>CHL4</t>
+          <t>CHL5</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>12062</v>
+        <v>1131</v>
       </c>
       <c r="C39" t="n">
-        <v>287415</v>
+        <v>24783</v>
       </c>
       <c r="D39" t="n">
-        <v>9.861925406003138</v>
+        <v>0.1791259240053478</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -1380,116 +1380,116 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>CHL5</t>
+          <t>CHL6</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>1131</v>
+        <v>21037</v>
       </c>
       <c r="C40" t="n">
-        <v>24783</v>
+        <v>3989467</v>
       </c>
       <c r="D40" t="n">
-        <v>0.503128235002805</v>
+        <v>26.52379394799937</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>COMPLETE</t>
+          <t>TIMEOUT</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>CHL6</t>
+          <t>CHL7</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>21037</v>
+        <v>26109</v>
       </c>
       <c r="C41" t="n">
-        <v>3989467</v>
+        <v>6497355</v>
       </c>
       <c r="D41" t="n">
-        <v>79.18678862099841</v>
+        <v>71.77097530799801</v>
       </c>
       <c r="E41" t="n">
         <v>6</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>TIMEOUT</t>
+          <t>COMPLETE</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>CHL7</t>
+          <t>Hchl1</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>26109</v>
+        <v>21037</v>
       </c>
       <c r="C42" t="n">
-        <v>6497355</v>
+        <v>3989467</v>
       </c>
       <c r="D42" t="n">
-        <v>337.9468957319987</v>
+        <v>26.48783655300213</v>
       </c>
       <c r="E42" t="n">
         <v>6</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>COMPLETE</t>
+          <t>TIMEOUT</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Hchl1</t>
+          <t>Hchl2</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>21037</v>
+        <v>26049</v>
       </c>
       <c r="C43" t="n">
-        <v>3989467</v>
+        <v>6470655</v>
       </c>
       <c r="D43" t="n">
-        <v>168.9720464689999</v>
+        <v>83.65945453500171</v>
       </c>
       <c r="E43" t="n">
         <v>6</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>TIMEOUT</t>
+          <t>COMPLETE</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Hchl2</t>
+          <t>Hchl3s</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>26049</v>
+        <v>14170</v>
       </c>
       <c r="C44" t="n">
-        <v>6470655</v>
+        <v>1350700</v>
       </c>
       <c r="D44" t="n">
-        <v>559.9519268339973</v>
+        <v>13.45013016500161</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -1500,20 +1500,20 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Hchl3s</t>
+          <t>Hchl4s</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>14170</v>
+        <v>7598</v>
       </c>
       <c r="C45" t="n">
-        <v>1350700</v>
+        <v>350770</v>
       </c>
       <c r="D45" t="n">
-        <v>43.94648537900139</v>
+        <v>3.603140851999342</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -1524,20 +1524,20 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Hchl4s</t>
+          <t>Hchl5s</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>7598</v>
+        <v>27280</v>
       </c>
       <c r="C46" t="n">
-        <v>350770</v>
+        <v>4738380</v>
       </c>
       <c r="D46" t="n">
-        <v>13.47172727500219</v>
+        <v>47.51820178899652</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -1548,20 +1548,20 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Hchl5s</t>
+          <t>Hchl6s</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>27280</v>
+        <v>29417</v>
       </c>
       <c r="C47" t="n">
-        <v>4738380</v>
+        <v>6532942</v>
       </c>
       <c r="D47" t="n">
-        <v>269.9323040169984</v>
+        <v>65.66112957699806</v>
       </c>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -1572,20 +1572,20 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Hchl6s</t>
+          <t>Hchl7s</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>29417</v>
+        <v>50118</v>
       </c>
       <c r="C48" t="n">
-        <v>6532942</v>
+        <v>20915127</v>
       </c>
       <c r="D48" t="n">
-        <v>167.621531697</v>
+        <v>297.2384830459996</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -1596,44 +1596,44 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Hchl7s</t>
+          <t>Hchl8s</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>50118</v>
+        <v>1617</v>
       </c>
       <c r="C49" t="n">
-        <v>20915127</v>
+        <v>17937</v>
       </c>
       <c r="D49" t="n">
-        <v>491.962087347</v>
+        <v>390.8667347299997</v>
       </c>
       <c r="E49" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>TIMEOUT</t>
+          <t>COMPLETE</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Hchl8s</t>
+          <t>Hchl9</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>1617</v>
+        <v>19375</v>
       </c>
       <c r="C50" t="n">
-        <v>17937</v>
+        <v>5451829</v>
       </c>
       <c r="D50" t="n">
-        <v>706.8403207309998</v>
+        <v>123.0014756040036</v>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -1644,20 +1644,20 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Hchl9</t>
+          <t>CHL2</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>19375</v>
+        <v>2242</v>
       </c>
       <c r="C51" t="n">
-        <v>5451829</v>
+        <v>83220</v>
       </c>
       <c r="D51" t="n">
-        <v>266.0364316330001</v>
+        <v>0.2611286970000037</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>

</xml_diff>